<commit_message>
automatically get  od pairs & try shotest path
</commit_message>
<xml_diff>
--- a/notebooks/train_stations.xlsx
+++ b/notebooks/train_stations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>geometry</t>
         </is>
       </c>
@@ -463,6 +468,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Diemen Zuid</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>POINT (4.9560598 52.3302613)</t>
         </is>
       </c>
@@ -480,6 +490,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Amstelveenseweg</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>POINT (4.8575769 52.3384028)</t>
         </is>
       </c>
@@ -497,6 +512,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Jan van Galenstraat</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>POINT (4.8352937 52.3726582)</t>
         </is>
       </c>
@@ -514,6 +534,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Amsterdam Holendrecht</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>POINT (4.9601712 52.2979886)</t>
         </is>
       </c>
@@ -531,6 +556,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Van der Madeweg</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>POINT (4.9305189 52.3294483)</t>
         </is>
       </c>
@@ -548,6 +578,11 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Overamstel</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>POINT (4.9176266 52.3317318)</t>
         </is>
       </c>
@@ -565,6 +600,11 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Halfweg-Zwanenburg</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>POINT (4.7468736 52.3859763)</t>
         </is>
       </c>
@@ -582,6 +622,11 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>De Vlugtlaan</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>POINT (4.8382223 52.3796134)</t>
         </is>
       </c>
@@ -599,6 +644,11 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Amsterdam Sloterdijk</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>POINT (4.8381062 52.3890317)</t>
         </is>
       </c>
@@ -616,6 +666,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>Amsterdam Bijlmer ArenA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>POINT (4.9470883 52.3122449)</t>
         </is>
       </c>
@@ -633,6 +688,11 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>Amsterdam Amstel</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>POINT (4.9175567 52.3464656)</t>
         </is>
       </c>
@@ -650,6 +710,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Gein</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>POINT (4.9890129 52.296338)</t>
         </is>
       </c>
@@ -667,6 +732,11 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>Reigersbos</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>POINT (4.9744218 52.2956478)</t>
         </is>
       </c>
@@ -684,6 +754,11 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>Gaasperplas</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>POINT (4.9843223 52.3113175)</t>
         </is>
       </c>
@@ -701,6 +776,11 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>Ganzenhoef</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>POINT (4.9735502 52.3230792)</t>
         </is>
       </c>
@@ -718,6 +798,11 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>Kraaiennest</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>POINT (4.9791233 52.3170313)</t>
         </is>
       </c>
@@ -735,6 +820,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>Venserpolder</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>POINT (4.9463398 52.3267669)</t>
         </is>
       </c>
@@ -752,6 +842,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>Duivendrecht</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>POINT (4.9364854 52.3235282)</t>
         </is>
       </c>
@@ -769,6 +864,11 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>Amsterdam RAI</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>POINT (4.8902289 52.3370349)</t>
         </is>
       </c>
@@ -786,6 +886,11 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>Strandvliet</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>POINT (4.9413557 52.3185355)</t>
         </is>
       </c>
@@ -803,6 +908,11 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>Bullewijk</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>POINT (4.9522364 52.3066107)</t>
         </is>
       </c>
@@ -820,6 +930,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>Heemstedestraat</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>POINT (4.8343026 52.3524713)</t>
         </is>
       </c>
@@ -837,6 +952,11 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>Verrijn Stuartweg</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>POINT (4.9662522 52.328939)</t>
         </is>
       </c>
@@ -854,6 +974,11 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Spaklerweg</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>POINT (4.9210115 52.3399595)</t>
         </is>
       </c>
@@ -871,6 +996,11 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>Wibautstraat</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>POINT (4.9120253 52.3544624)</t>
         </is>
       </c>
@@ -888,6 +1018,11 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>Nieuwmarkt</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>POINT (4.9008788 52.3713176)</t>
         </is>
       </c>
@@ -905,6 +1040,11 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>Henk Sneevlietweg</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>POINT (4.8345025 52.3464029)</t>
         </is>
       </c>
@@ -922,6 +1062,11 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Amsterdam Lelylaan</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>POINT (4.8340268 52.3578369)</t>
         </is>
       </c>
@@ -939,6 +1084,11 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>Isolatorweg</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>POINT (4.8507911 52.3951713)</t>
         </is>
       </c>
@@ -956,6 +1106,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>Postjesweg</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t>POINT (4.8339612 52.3642921)</t>
         </is>
       </c>
@@ -973,6 +1128,11 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>Zaandam</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>POINT (4.8137421 52.4382493)</t>
         </is>
       </c>
@@ -990,6 +1150,11 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>Amsterdam Centraal</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>POINT (4.9005805 52.378901)</t>
         </is>
       </c>
@@ -1007,6 +1172,11 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Amsterdam Muiderpoort</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>POINT (4.9311934 52.3608341)</t>
         </is>
       </c>
@@ -1024,6 +1194,11 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>Amsterdam Zuid</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>POINT (4.8734324 52.3390172)</t>
         </is>
       </c>
@@ -1041,6 +1216,11 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>Zuid</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>POINT (4.8744481 52.3391807)</t>
         </is>
       </c>
@@ -1058,6 +1238,11 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>Station Sloterdijk</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>POINT (4.838877 52.3890161)</t>
         </is>
       </c>
@@ -1075,6 +1260,11 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>Station RAI</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>POINT (4.8893261 52.3377124)</t>
         </is>
       </c>
@@ -1092,6 +1282,11 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>Centraal Station</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>POINT (4.9009578 52.3774316)</t>
         </is>
       </c>
@@ -1109,6 +1304,11 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>Europaplein</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>POINT (4.8914727 52.3416064)</t>
         </is>
       </c>
@@ -1126,6 +1326,11 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>De Pijp</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>POINT (4.8906926 52.3539754)</t>
         </is>
       </c>
@@ -1143,6 +1348,11 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>Vijzelgracht</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>POINT (4.8911097 52.3606741)</t>
         </is>
       </c>
@@ -1160,6 +1370,11 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>Noorderpark</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>POINT (4.9187004 52.3889316)</t>
         </is>
       </c>
@@ -1177,6 +1392,11 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>Noord</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>POINT (4.9323589 52.4019931)</t>
         </is>
       </c>
@@ -1194,6 +1414,11 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>Amsterdam Science Park</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>POINT (4.948315 52.352926)</t>
         </is>
       </c>
@@ -1211,6 +1436,11 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>Diemen</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>POINT (4.9674386 52.345214)</t>
         </is>
       </c>
@@ -1227,6 +1457,11 @@
         </is>
       </c>
       <c r="C47" t="inlineStr">
+        <is>
+          <t>Centraal Station</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
         <is>
           <t>POINT (4.9009058 52.3791977)</t>
         </is>

</xml_diff>